<commit_message>
Añadir formulario de informe en la sección 1
</commit_message>
<xml_diff>
--- a/app/tables/tabla_lagrange.xlsx
+++ b/app/tables/tabla_lagrange.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -443,7 +443,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Inf -Inf </t>
+          <t xml:space="preserve">-1.300000 1.500000 5.200000 </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Organiza los splines y las celdas de la sección 3
</commit_message>
<xml_diff>
--- a/app/tables/tabla_lagrange.xlsx
+++ b/app/tables/tabla_lagrange.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -443,7 +443,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">-1.300000 1.500000 5.200000 </t>
+          <t>(4824*x^2)/51935 - (37958*x)/51935 + 20984/10387</t>
         </is>
       </c>
     </row>

</xml_diff>